<commit_message>
Remove Backspace Function Key
</commit_message>
<xml_diff>
--- a/CL Hotkey.xlsx
+++ b/CL Hotkey.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\@TEMP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Files\Projects\GitHub\CapsLite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD5741B2-1220-4911-BF21-FE9249A2AC66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22362D9E-0A29-4C97-948C-7B6E1FCE187E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="253">
   <si>
     <t>Alphabet</t>
   </si>
@@ -97,9 +97,6 @@
     <t>Ctrl Alt F1</t>
   </si>
   <si>
-    <t>Alt Shift F1</t>
-  </si>
-  <si>
     <t>F2</t>
   </si>
   <si>
@@ -124,9 +121,6 @@
     <t>Ctrl Alt F2</t>
   </si>
   <si>
-    <t>Alt Shift F2</t>
-  </si>
-  <si>
     <t>F3</t>
   </si>
   <si>
@@ -151,9 +145,6 @@
     <t>Ctrl Alt F3</t>
   </si>
   <si>
-    <t>Alt Shift F3</t>
-  </si>
-  <si>
     <t>F4</t>
   </si>
   <si>
@@ -178,9 +169,6 @@
     <t>Ctrl Alt F4</t>
   </si>
   <si>
-    <t>Alt Shift F4</t>
-  </si>
-  <si>
     <t>F5</t>
   </si>
   <si>
@@ -205,9 +193,6 @@
     <t>Ctrl Alt F5</t>
   </si>
   <si>
-    <t>Alt Shift F5</t>
-  </si>
-  <si>
     <t>F6</t>
   </si>
   <si>
@@ -232,9 +217,6 @@
     <t>Ctrl Alt F6</t>
   </si>
   <si>
-    <t>Alt Shift F6</t>
-  </si>
-  <si>
     <t>F7</t>
   </si>
   <si>
@@ -259,9 +241,6 @@
     <t>Ctrl Alt F7</t>
   </si>
   <si>
-    <t>Alt Shift F7</t>
-  </si>
-  <si>
     <t>F8</t>
   </si>
   <si>
@@ -286,9 +265,6 @@
     <t>Ctrl Alt F8</t>
   </si>
   <si>
-    <t>Alt Shift F8</t>
-  </si>
-  <si>
     <t>F9</t>
   </si>
   <si>
@@ -313,9 +289,6 @@
     <t>Ctrl Alt F9</t>
   </si>
   <si>
-    <t>Alt Shift F9</t>
-  </si>
-  <si>
     <t>F10</t>
   </si>
   <si>
@@ -340,9 +313,6 @@
     <t>Ctrl Alt F10</t>
   </si>
   <si>
-    <t>Alt Shift F10</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -370,9 +340,6 @@
     <t>Ctrl Alt F11</t>
   </si>
   <si>
-    <t>Alt Shift F11</t>
-  </si>
-  <si>
     <t>=</t>
   </si>
   <si>
@@ -398,9 +365,6 @@
   </si>
   <si>
     <t>Ctrl Alt F12</t>
-  </si>
-  <si>
-    <t>Alt Shift F12</t>
   </si>
   <si>
     <t>+</t>
@@ -774,6 +738,62 @@
   </si>
   <si>
     <t>`</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Caps Alt</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alt Shift F1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alt Shift F2</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alt Shift F3</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alt Shift F4</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alt Shift F5</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alt Shift F6</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alt Shift F7</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alt Shift F8</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alt Shift F9</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alt Shift F10</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alt Shift F11</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alt Shift F12</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>\ &amp; ]</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
@@ -781,7 +801,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -886,6 +906,24 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF7C80"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -945,7 +983,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1031,6 +1069,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1379,8 +1423,8 @@
       <c r="L2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="6" t="s">
-        <v>12</v>
+      <c r="M2" s="30" t="s">
+        <v>252</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>13</v>
@@ -1440,9 +1484,7 @@
       <c r="M4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="N4" s="8" t="s">
-        <v>14</v>
-      </c>
+      <c r="N4" s="20"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -1522,11 +1564,11 @@
       <c r="K6" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="L6" s="29" t="s">
+        <v>240</v>
+      </c>
+      <c r="M6" s="11" t="s">
         <v>24</v>
-      </c>
-      <c r="M6" s="11" t="s">
-        <v>25</v>
       </c>
       <c r="N6" s="8" t="s">
         <v>14</v>
@@ -1543,34 +1585,34 @@
         <v>2</v>
       </c>
       <c r="D7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="11" t="s">
+      <c r="G7" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="H7" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="I7" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="J7" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="J7" s="11" t="s">
+      <c r="K7" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="K7" s="11" t="s">
+      <c r="L7" s="29" t="s">
+        <v>241</v>
+      </c>
+      <c r="M7" s="11" t="s">
         <v>32</v>
-      </c>
-      <c r="L7" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="M7" s="11" t="s">
-        <v>34</v>
       </c>
       <c r="N7" s="8" t="s">
         <v>14</v>
@@ -1587,34 +1629,34 @@
         <v>3</v>
       </c>
       <c r="D8" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="11" t="s">
+      <c r="H8" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="I8" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="J8" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="K8" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="L8" s="29" t="s">
+        <v>242</v>
+      </c>
+      <c r="M8" s="11" t="s">
         <v>40</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="L8" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="M8" s="11" t="s">
-        <v>43</v>
       </c>
       <c r="N8" s="8" t="s">
         <v>14</v>
@@ -1631,34 +1673,34 @@
         <v>4</v>
       </c>
       <c r="D9" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="11" t="s">
+      <c r="I9" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="J9" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="K9" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="L9" s="29" t="s">
+        <v>243</v>
+      </c>
+      <c r="M9" s="11" t="s">
         <v>48</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="K9" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="L9" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="M9" s="11" t="s">
-        <v>52</v>
       </c>
       <c r="N9" s="8" t="s">
         <v>14</v>
@@ -1675,34 +1717,34 @@
         <v>5</v>
       </c>
       <c r="D10" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="I10" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="11" t="s">
+      <c r="J10" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="K10" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="H10" s="13" t="s">
+      <c r="L10" s="29" t="s">
+        <v>244</v>
+      </c>
+      <c r="M10" s="11" t="s">
         <v>56</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="J10" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="K10" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="L10" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="M10" s="11" t="s">
-        <v>61</v>
       </c>
       <c r="N10" s="8" t="s">
         <v>14</v>
@@ -1719,34 +1761,34 @@
         <v>6</v>
       </c>
       <c r="D11" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J11" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="11" t="s">
+      <c r="K11" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="L11" s="29" t="s">
+        <v>245</v>
+      </c>
+      <c r="M11" s="11" t="s">
         <v>64</v>
-      </c>
-      <c r="H11" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="J11" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="K11" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="L11" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="M11" s="11" t="s">
-        <v>70</v>
       </c>
       <c r="N11" s="8" t="s">
         <v>14</v>
@@ -1763,34 +1805,34 @@
         <v>7</v>
       </c>
       <c r="D12" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="K12" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="11" t="s">
+      <c r="L12" s="29" t="s">
+        <v>246</v>
+      </c>
+      <c r="M12" s="11" t="s">
         <v>72</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="H12" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="J12" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="K12" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="L12" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="M12" s="11" t="s">
-        <v>79</v>
       </c>
       <c r="N12" s="13">
         <v>7</v>
@@ -1807,34 +1849,34 @@
         <v>8</v>
       </c>
       <c r="D13" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="L13" s="29" t="s">
+        <v>247</v>
+      </c>
+      <c r="M13" s="11" t="s">
         <v>80</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="H13" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="L13" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="M13" s="11" t="s">
-        <v>88</v>
       </c>
       <c r="N13" s="13">
         <v>8</v>
@@ -1851,34 +1893,34 @@
         <v>9</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>14</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="L14" s="11" t="s">
-        <v>96</v>
+        <v>87</v>
+      </c>
+      <c r="L14" s="29" t="s">
+        <v>248</v>
       </c>
       <c r="M14" s="11" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="N14" s="13">
         <v>9</v>
@@ -1895,37 +1937,37 @@
         <v>0</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>14</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="L15" s="11" t="s">
-        <v>105</v>
+        <v>95</v>
+      </c>
+      <c r="L15" s="29" t="s">
+        <v>249</v>
       </c>
       <c r="M15" s="11" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="N15" s="13" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -1936,40 +1978,40 @@
         <v>13</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>14</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="J16" s="11" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="K16" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="L16" s="11" t="s">
-        <v>115</v>
+        <v>104</v>
+      </c>
+      <c r="L16" s="29" t="s">
+        <v>250</v>
       </c>
       <c r="M16" s="11" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="N16" s="13" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -1980,40 +2022,40 @@
         <v>14</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>14</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="K17" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="L17" s="11" t="s">
-        <v>125</v>
+        <v>113</v>
+      </c>
+      <c r="L17" s="29" t="s">
+        <v>251</v>
       </c>
       <c r="M17" s="11" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="N17" s="13" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -2036,7 +2078,7 @@
         <v>14</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>14</v>
@@ -2053,10 +2095,10 @@
       <c r="L18" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M18" s="21"/>
-      <c r="N18" s="10" t="s">
-        <v>12</v>
-      </c>
+      <c r="M18" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="N18" s="23"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
@@ -2066,7 +2108,7 @@
         <v>16</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>14</v>
@@ -2095,10 +2137,10 @@
       <c r="L19" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M19" s="21"/>
-      <c r="N19" s="23" t="s">
-        <v>129</v>
-      </c>
+      <c r="M19" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="N19" s="23"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
@@ -2140,7 +2182,7 @@
         <v>14</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>14</v>
@@ -2158,9 +2200,7 @@
       <c r="M21" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="N21" s="8" t="s">
-        <v>14</v>
-      </c>
+      <c r="N21" s="20"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
@@ -2170,7 +2210,7 @@
         <v>19</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>8</v>
@@ -2179,13 +2219,13 @@
         <v>14</v>
       </c>
       <c r="F22" s="18" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>14</v>
       </c>
       <c r="H22" s="28" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="I22" s="8" t="s">
         <v>14</v>
@@ -2214,28 +2254,28 @@
         <v>20</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="F23" s="17" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="G23" s="8" t="s">
         <v>14</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="I23" s="8" t="s">
         <v>14</v>
       </c>
       <c r="J23" s="19" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="K23" s="8" t="s">
         <v>14</v>
@@ -2258,22 +2298,22 @@
         <v>21</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="F24" s="18" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>14</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="I24" s="8" t="s">
         <v>14</v>
@@ -2302,16 +2342,16 @@
         <v>22</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="F25" s="18" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="G25" s="8" t="s">
         <v>14</v>
@@ -2320,7 +2360,7 @@
         <v>20</v>
       </c>
       <c r="I25" s="19" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="J25" s="8" t="s">
         <v>14</v>
@@ -2346,22 +2386,22 @@
         <v>23</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="F26" s="17" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="G26" s="8" t="s">
         <v>14</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="I26" s="8" t="s">
         <v>14</v>
@@ -2390,22 +2430,22 @@
         <v>24</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="F27" s="18" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="G27" s="8" t="s">
         <v>14</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="I27" s="8" t="s">
         <v>14</v>
@@ -2434,13 +2474,13 @@
         <v>25</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="F28" s="8" t="s">
         <v>14</v>
@@ -2449,7 +2489,7 @@
         <v>14</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="I28" s="8" t="s">
         <v>14</v>
@@ -2478,22 +2518,22 @@
         <v>26</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="F29" s="18" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>14</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="I29" s="8" t="s">
         <v>14</v>
@@ -2522,22 +2562,22 @@
         <v>27</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="F30" s="18" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>14</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="I30" s="8" t="s">
         <v>14</v>
@@ -2566,16 +2606,16 @@
         <v>28</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>14</v>
@@ -2599,7 +2639,7 @@
         <v>14</v>
       </c>
       <c r="N31" s="13" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -2610,13 +2650,13 @@
         <v>29</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>14</v>
@@ -2643,7 +2683,7 @@
         <v>14</v>
       </c>
       <c r="N32" s="13" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -2657,10 +2697,10 @@
         <v>11</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>14</v>
@@ -2681,11 +2721,9 @@
         <v>14</v>
       </c>
       <c r="L33" s="21"/>
-      <c r="M33" s="8" t="s">
-        <v>14</v>
-      </c>
+      <c r="M33" s="21"/>
       <c r="N33" s="13" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -2702,7 +2740,7 @@
         <v>10</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>14</v>
@@ -2721,9 +2759,7 @@
       </c>
       <c r="K34" s="21"/>
       <c r="L34" s="21"/>
-      <c r="M34" s="8" t="s">
-        <v>14</v>
-      </c>
+      <c r="M34" s="21"/>
       <c r="N34" s="13" t="s">
         <v>10</v>
       </c>
@@ -2780,7 +2816,7 @@
         <v>34</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>14</v>
@@ -2793,7 +2829,7 @@
         <v>14</v>
       </c>
       <c r="H37" s="13" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="I37" s="8" t="s">
         <v>14</v>
@@ -2822,22 +2858,22 @@
         <v>35</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="D38" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="F38" s="17" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>14</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="I38" s="8" t="s">
         <v>14</v>
@@ -2866,22 +2902,22 @@
         <v>36</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="F39" s="22" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="G39" s="8" t="s">
         <v>14</v>
       </c>
       <c r="H39" s="13" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="I39" s="8" t="s">
         <v>14</v>
@@ -2910,22 +2946,22 @@
         <v>37</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="F40" s="22" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="G40" s="8" t="s">
         <v>14</v>
       </c>
       <c r="H40" s="13" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="I40" s="8" t="s">
         <v>14</v>
@@ -2954,22 +2990,22 @@
         <v>38</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="F41" s="22" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="G41" s="8" t="s">
         <v>14</v>
       </c>
       <c r="H41" s="13" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="I41" s="8" t="s">
         <v>14</v>
@@ -2998,28 +3034,28 @@
         <v>39</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="F42" s="12" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="G42" s="8" t="s">
         <v>14</v>
       </c>
       <c r="H42" s="13" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="I42" s="19" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="J42" s="19" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="K42" s="8" t="s">
         <v>14</v>
@@ -3042,28 +3078,28 @@
         <v>40</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="F43" s="22" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="G43" s="8" t="s">
         <v>14</v>
       </c>
       <c r="H43" s="13" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="I43" s="19" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="J43" s="19" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="K43" s="8" t="s">
         <v>14</v>
@@ -3086,28 +3122,28 @@
         <v>41</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="F44" s="22" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="G44" s="8" t="s">
         <v>14</v>
       </c>
       <c r="H44" s="13" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="I44" s="19" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="J44" s="19" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="K44" s="8" t="s">
         <v>14</v>
@@ -3130,28 +3166,28 @@
         <v>42</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="F45" s="12" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="G45" s="8" t="s">
         <v>14</v>
       </c>
       <c r="H45" s="13" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="I45" s="19" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="J45" s="19" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="K45" s="8" t="s">
         <v>14</v>
@@ -3174,19 +3210,19 @@
         <v>43</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="F46" s="8" t="s">
         <v>14</v>
       </c>
       <c r="G46" s="12" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="H46" s="21"/>
       <c r="I46" s="8" t="s">
@@ -3205,7 +3241,7 @@
         <v>14</v>
       </c>
       <c r="N46" s="13" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
@@ -3216,13 +3252,13 @@
         <v>44</v>
       </c>
       <c r="C47" s="24" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="D47" s="25" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="E47" s="25" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="F47" s="8" t="s">
         <v>14</v>
@@ -3249,7 +3285,7 @@
         <v>14</v>
       </c>
       <c r="N47" s="25" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
@@ -3260,7 +3296,7 @@
         <v>45</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>14</v>
@@ -3269,10 +3305,10 @@
         <v>14</v>
       </c>
       <c r="F48" s="26" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="G48" s="27" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="H48" s="8" t="s">
         <v>14</v>
@@ -3292,9 +3328,7 @@
       <c r="M48" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="N48" s="10" t="s">
-        <v>145</v>
-      </c>
+      <c r="N48" s="10"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
@@ -3324,10 +3358,10 @@
         <v>47</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="E50" s="8" t="s">
         <v>14</v>
@@ -3339,7 +3373,7 @@
         <v>14</v>
       </c>
       <c r="H50" s="13" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="I50" s="8" t="s">
         <v>14</v>
@@ -3368,13 +3402,13 @@
         <v>48</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="F51" s="8" t="s">
         <v>14</v>
@@ -3412,13 +3446,13 @@
         <v>49</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="E52" s="17" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="F52" s="8" t="s">
         <v>14</v>
@@ -3427,7 +3461,7 @@
         <v>14</v>
       </c>
       <c r="H52" s="13" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="I52" s="8" t="s">
         <v>14</v>
@@ -3456,13 +3490,13 @@
         <v>50</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="F53" s="8" t="s">
         <v>14</v>
@@ -3471,7 +3505,7 @@
         <v>14</v>
       </c>
       <c r="H53" s="13" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="I53" s="8" t="s">
         <v>14</v>
@@ -3500,13 +3534,13 @@
         <v>51</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="F54" s="8" t="s">
         <v>14</v>
@@ -3515,7 +3549,7 @@
         <v>14</v>
       </c>
       <c r="H54" s="13" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="I54" s="8" t="s">
         <v>14</v>
@@ -3544,13 +3578,13 @@
         <v>52</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="F55" s="8" t="s">
         <v>14</v>
@@ -3559,7 +3593,7 @@
         <v>14</v>
       </c>
       <c r="H55" s="13" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="I55" s="8" t="s">
         <v>14</v>
@@ -3588,13 +3622,13 @@
         <v>53</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="F56" s="8" t="s">
         <v>14</v>
@@ -3603,7 +3637,7 @@
         <v>14</v>
       </c>
       <c r="H56" s="13" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="I56" s="8" t="s">
         <v>14</v>
@@ -3632,13 +3666,13 @@
         <v>54</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="D57" s="13" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="E57" s="13" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="F57" s="8" t="s">
         <v>14</v>
@@ -3647,7 +3681,7 @@
         <v>14</v>
       </c>
       <c r="H57" s="13" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="I57" s="8" t="s">
         <v>14</v>
@@ -3665,7 +3699,7 @@
         <v>14</v>
       </c>
       <c r="N57" s="13" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
@@ -3676,13 +3710,13 @@
         <v>55</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="D58" s="13" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="E58" s="13" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="F58" s="8" t="s">
         <v>14</v>
@@ -3709,7 +3743,7 @@
         <v>14</v>
       </c>
       <c r="N58" s="13" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
@@ -3720,13 +3754,13 @@
         <v>56</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="D59" s="13" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="E59" s="13" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="F59" s="8" t="s">
         <v>14</v>
@@ -3753,7 +3787,7 @@
         <v>14</v>
       </c>
       <c r="N59" s="13" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
@@ -3792,9 +3826,7 @@
       <c r="M60" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="N60" s="10" t="s">
-        <v>6</v>
-      </c>
+      <c r="N60" s="10"/>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="7">

</xml_diff>

<commit_message>
Fix the Semicolon bug
</commit_message>
<xml_diff>
--- a/CL Hotkey.xlsx
+++ b/CL Hotkey.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Files\Projects\GitHub\CapsLite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22362D9E-0A29-4C97-948C-7B6E1FCE187E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A749051B-55B5-4315-BAB4-1E919C8812EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="252">
   <si>
     <t>Alphabet</t>
   </si>
@@ -738,10 +738,6 @@
   </si>
   <si>
     <t>`</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Caps Alt</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
@@ -1424,7 +1420,7 @@
         <v>11</v>
       </c>
       <c r="M2" s="30" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>13</v>
@@ -1565,7 +1561,7 @@
         <v>23</v>
       </c>
       <c r="L6" s="29" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M6" s="11" t="s">
         <v>24</v>
@@ -1609,7 +1605,7 @@
         <v>31</v>
       </c>
       <c r="L7" s="29" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="M7" s="11" t="s">
         <v>32</v>
@@ -1653,7 +1649,7 @@
         <v>39</v>
       </c>
       <c r="L8" s="29" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M8" s="11" t="s">
         <v>40</v>
@@ -1697,7 +1693,7 @@
         <v>47</v>
       </c>
       <c r="L9" s="29" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="M9" s="11" t="s">
         <v>48</v>
@@ -1741,7 +1737,7 @@
         <v>55</v>
       </c>
       <c r="L10" s="29" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M10" s="11" t="s">
         <v>56</v>
@@ -1785,7 +1781,7 @@
         <v>63</v>
       </c>
       <c r="L11" s="29" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="M11" s="11" t="s">
         <v>64</v>
@@ -1829,7 +1825,7 @@
         <v>71</v>
       </c>
       <c r="L12" s="29" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="M12" s="11" t="s">
         <v>72</v>
@@ -1873,7 +1869,7 @@
         <v>79</v>
       </c>
       <c r="L13" s="29" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="M13" s="11" t="s">
         <v>80</v>
@@ -1917,7 +1913,7 @@
         <v>87</v>
       </c>
       <c r="L14" s="29" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="M14" s="11" t="s">
         <v>88</v>
@@ -1961,7 +1957,7 @@
         <v>95</v>
       </c>
       <c r="L15" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="M15" s="11" t="s">
         <v>96</v>
@@ -2005,7 +2001,7 @@
         <v>104</v>
       </c>
       <c r="L16" s="29" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="M16" s="11" t="s">
         <v>105</v>
@@ -2049,7 +2045,7 @@
         <v>113</v>
       </c>
       <c r="L17" s="29" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="M17" s="11" t="s">
         <v>114</v>
@@ -2362,8 +2358,8 @@
       <c r="I25" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="J25" s="8" t="s">
-        <v>14</v>
+      <c r="J25" s="12" t="s">
+        <v>210</v>
       </c>
       <c r="K25" s="8" t="s">
         <v>14</v>
@@ -3221,8 +3217,8 @@
       <c r="F46" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G46" s="12" t="s">
-        <v>210</v>
+      <c r="G46" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="H46" s="21"/>
       <c r="I46" s="8" t="s">

</xml_diff>